<commit_message>
debug display part done
</commit_message>
<xml_diff>
--- a/Documentation/Layout.xlsx
+++ b/Documentation/Layout.xlsx
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -197,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +230,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -534,185 +555,191 @@
   <dimension ref="A1:AQ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="2.5703125" style="2"/>
+    <col min="1" max="1" width="3" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.5703125" style="2" customWidth="1"/>
+    <col min="23" max="43" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="2.5703125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7">
         <f>B1+1</f>
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="7">
         <f t="shared" ref="D1:AQ1" si="0">C1+1</f>
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="7">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="7">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="X1" s="2">
+      <c r="X1" s="7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="Y1" s="7">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Z1" s="7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AA1" s="7">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AB1" s="7">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AC1" s="2">
+      <c r="AC1" s="7">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AD1" s="2">
+      <c r="AD1" s="7">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AE1" s="2">
+      <c r="AE1" s="7">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AF1" s="7">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AG1" s="2">
+      <c r="AG1" s="7">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AH1" s="7">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AI1" s="2">
+      <c r="AI1" s="7">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AJ1" s="2">
+      <c r="AJ1" s="7">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AK1" s="2">
+      <c r="AK1" s="7">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AL1" s="2">
+      <c r="AL1" s="7">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AM1" s="2">
+      <c r="AM1" s="7">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AN1" s="2">
+      <c r="AN1" s="7">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AO1" s="2">
+      <c r="AO1" s="7">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AP1" s="2">
+      <c r="AP1" s="7">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AQ1" s="2">
+      <c r="AQ1" s="7">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="8">
         <v>0</v>
       </c>
       <c r="B2" s="3">
@@ -811,7 +838,7 @@
       </c>
     </row>
     <row r="3" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="8">
         <f>A2+1</f>
         <v>1</v>
       </c>
@@ -901,7 +928,7 @@
       </c>
     </row>
     <row r="4" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="8">
         <f t="shared" ref="A4:A26" si="1">A3+1</f>
         <v>2</v>
       </c>
@@ -1001,7 +1028,7 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="8">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1093,7 +1120,7 @@
       <c r="AQ5" s="1"/>
     </row>
     <row r="6" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1169,7 +1196,7 @@
       <c r="AQ6" s="1"/>
     </row>
     <row r="7" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1277,7 +1304,7 @@
       </c>
     </row>
     <row r="8" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="8">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1383,7 +1410,7 @@
       </c>
     </row>
     <row r="9" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="8">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -1489,7 +1516,7 @@
       </c>
     </row>
     <row r="10" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -1595,7 +1622,7 @@
       </c>
     </row>
     <row r="11" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -1701,7 +1728,7 @@
       </c>
     </row>
     <row r="12" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="8">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -1807,7 +1834,7 @@
       </c>
     </row>
     <row r="13" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="8">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -1913,7 +1940,7 @@
       </c>
     </row>
     <row r="14" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="8">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -2003,7 +2030,7 @@
       <c r="AQ14" s="1"/>
     </row>
     <row r="15" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="A15" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -2093,7 +2120,7 @@
       <c r="AQ15" s="1"/>
     </row>
     <row r="16" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="A16" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
@@ -2183,7 +2210,7 @@
       <c r="AQ16" s="1"/>
     </row>
     <row r="17" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -2273,7 +2300,7 @@
       <c r="AQ17" s="1"/>
     </row>
     <row r="18" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="A18" s="8">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -2321,7 +2348,7 @@
       <c r="AQ18" s="1"/>
     </row>
     <row r="19" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="A19" s="8">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -2443,7 +2470,7 @@
       </c>
     </row>
     <row r="20" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="A20" s="8">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -2565,7 +2592,7 @@
       </c>
     </row>
     <row r="21" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="A21" s="8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -2687,7 +2714,7 @@
       </c>
     </row>
     <row r="22" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="A22" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -2809,7 +2836,7 @@
       </c>
     </row>
     <row r="23" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="A23" s="8">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
@@ -2931,7 +2958,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="A24" s="8">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
@@ -3053,7 +3080,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="A25" s="8">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
@@ -3175,7 +3202,7 @@
       </c>
     </row>
     <row r="26" spans="1:43" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="A26" s="8">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>

</xml_diff>